<commit_message>
Update DB - add new column to Items
</commit_message>
<xml_diff>
--- a/Design/CSDL.xlsx
+++ b/Design/CSDL.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Staff</t>
   </si>
@@ -76,6 +76,15 @@
     <t>delivered</t>
   </si>
   <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>0-7</t>
+  </si>
+  <si>
+    <t>description: SML=111binary=7, SML=011binary=3,....</t>
+  </si>
+  <si>
     <t>hashed pw</t>
   </si>
   <si>
@@ -85,6 +94,12 @@
     <t>delivering</t>
   </si>
   <si>
+    <t>ice</t>
+  </si>
+  <si>
+    <t>0-disable, 1-enable</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
@@ -92,6 +107,9 @@
   </si>
   <si>
     <t>on-hold</t>
+  </si>
+  <si>
+    <t>sugar</t>
   </si>
   <si>
     <t>staff</t>
@@ -140,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -155,11 +173,15 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FFFFFF00"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +220,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF990000"/>
         <bgColor rgb="FF990000"/>
       </patternFill>
@@ -215,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border/>
     <border>
       <left style="thin">
@@ -267,12 +295,59 @@
       </top>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
       <left style="dotted">
         <color rgb="FF000000"/>
       </left>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
       <right style="dotted">
         <color rgb="FF000000"/>
       </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="dotted">
@@ -289,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -323,19 +398,36 @@
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="12" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -559,6 +651,8 @@
   <cols>
     <col customWidth="1" min="4" max="4" width="14.14"/>
     <col customWidth="1" min="7" max="7" width="17.14"/>
+    <col customWidth="1" min="11" max="11" width="17.14"/>
+    <col customWidth="1" min="12" max="12" width="54.29"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -656,7 +750,7 @@
       <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -673,54 +767,77 @@
       <c r="G8" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="J8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="15"/>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="G10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="18"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12">
-      <c r="G12" s="12" t="s">
-        <v>29</v>
+      <c r="G12" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>32</v>
+      <c r="B14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15">
@@ -728,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>5</v>
@@ -736,10 +853,10 @@
     </row>
     <row r="16">
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>8</v>
@@ -747,15 +864,15 @@
     </row>
     <row r="17">
       <c r="B17" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>11</v>
@@ -766,26 +883,26 @@
         <v>19</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="16"/>
+      <c r="B20" s="23"/>
       <c r="G20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21">
-      <c r="H21" s="10" t="s">
-        <v>28</v>
+      <c r="H21" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22">
-      <c r="H22" s="12" t="s">
-        <v>26</v>
+      <c r="H22" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>